<commit_message>
Updating TP for PS (ready)
</commit_message>
<xml_diff>
--- a/Docs/Tarea5-6/TP-BAT.xlsx
+++ b/Docs/Tarea5-6/TP-BAT.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicsma2409\Desktop\Maestria\1er Cuatrimestre 2025\Verificacion\ProyectoFinal\Repo_SSH\Docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Vicsma2409\Desktop\Maestria\1er Cuatrimestre 2025\Verificacion\ProyectoFinal\Repo_SSH\Docs\Tarea5-6\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35845B8C-C872-48DE-B4C3-878125A65419}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E382045-FDF4-46F5-AD3D-C60EDCB790B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="21000" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="594" uniqueCount="184">
   <si>
     <t>ID</t>
   </si>
@@ -55,12 +55,6 @@
     <t>Entradas</t>
   </si>
   <si>
-    <t>#</t>
-  </si>
-  <si>
-    <t>Req. ID</t>
-  </si>
-  <si>
     <t>E1</t>
   </si>
   <si>
@@ -157,9 +151,6 @@
     <t>Valor obtenido</t>
   </si>
   <si>
-    <t>Los pasos de verificación tienen la forma: Verificar que &lt;variable de salida&gt; es igual que &lt;valor esperado.&gt;</t>
-  </si>
-  <si>
     <t>Ejecutado por</t>
   </si>
   <si>
@@ -169,9 +160,6 @@
     <t>TP-BAT</t>
   </si>
   <si>
-    <t>Borrador 5</t>
-  </si>
-  <si>
     <t>V.  Sanchez</t>
   </si>
   <si>
@@ -185,9 +173,6 @@
   </si>
   <si>
     <t>-</t>
-  </si>
-  <si>
-    <t>Falló</t>
   </si>
   <si>
     <t>Permitir la ejecución normal del programa.
@@ -227,15 +212,9 @@
     <t>Clase Equivalencia</t>
   </si>
   <si>
-    <t>Verifcar que el LED "Batería" es igual a apagado (no color)</t>
-  </si>
-  <si>
     <t>Mover el Nivel de Batería: 0</t>
   </si>
   <si>
-    <t>Verifcar que el LED "Batería" es igual a encendido (verde)</t>
-  </si>
-  <si>
     <t>APAGADO</t>
   </si>
   <si>
@@ -243,13 +222,436 @@
   </si>
   <si>
     <t>TP-BAT-002</t>
+  </si>
+  <si>
+    <t>Este paso determinará el valor límite de la batería de respaldo en caso de falla eléctrica</t>
+  </si>
+  <si>
+    <t>Seleccionar, en interfaz de simulación, opción "Sim falla PS Principal OFF"</t>
+  </si>
+  <si>
+    <t>Esta instrucción indica que la fuente de alimentación principal se encuentra funcional</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 100%</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 0%</t>
+  </si>
+  <si>
+    <t>Mover el Nivel de Batería: 20</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 20%</t>
+  </si>
+  <si>
+    <t>Mover el Nivel de Batería: 49</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 49%</t>
+  </si>
+  <si>
+    <t>Mover el Nivel de Batería: 50</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 50%</t>
+  </si>
+  <si>
+    <t>Mover el Nivel de Batería: 51</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 51%</t>
+  </si>
+  <si>
+    <t>Indica que la batería de respaldo se encuentra cargada al 80%</t>
+  </si>
+  <si>
+    <t>Mover el Nivel de Batería: 80</t>
+  </si>
+  <si>
+    <t>Seleccionar, en interfaz de simulación, opción "Sim falla PS Principal ON"</t>
+  </si>
+  <si>
+    <t>Esta instrucción indica que la fuente de alimentación principal NO se encuentra funcional</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" es igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Batería" ya que aunque el nivel de la batería de respaldo es mayor o igual que el límite establecido, la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" es igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" es igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" es igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>TP-BAT-003</t>
+  </si>
+  <si>
+    <t>TP-BAT-004</t>
+  </si>
+  <si>
+    <t>TP-BAT-005</t>
+  </si>
+  <si>
+    <t>TP-BAT-006</t>
+  </si>
+  <si>
+    <t>TP-BAT-007</t>
+  </si>
+  <si>
+    <t>TP-BAT-008</t>
+  </si>
+  <si>
+    <t>TP-BAT-009</t>
+  </si>
+  <si>
+    <t>TP-BAT-010</t>
+  </si>
+  <si>
+    <t>TP-BAT-011</t>
+  </si>
+  <si>
+    <t>TP-BAT-012</t>
+  </si>
+  <si>
+    <t>TP-BAT-013</t>
+  </si>
+  <si>
+    <t>TP-BAT-014</t>
+  </si>
+  <si>
+    <t>TP-BAT-015</t>
+  </si>
+  <si>
+    <t>TP-BAT-016</t>
+  </si>
+  <si>
+    <t>TP-BAT-017</t>
+  </si>
+  <si>
+    <t>TP-BAT-018</t>
+  </si>
+  <si>
+    <t>TP-BAT-019</t>
+  </si>
+  <si>
+    <t>TP-BAT-020</t>
+  </si>
+  <si>
+    <t>TP-BAT-021</t>
+  </si>
+  <si>
+    <t>TP-BAT-022</t>
+  </si>
+  <si>
+    <t>TP-BAT-023</t>
+  </si>
+  <si>
+    <t>TP-BAT-024</t>
+  </si>
+  <si>
+    <t>TP-BAT-025</t>
+  </si>
+  <si>
+    <t>TP-BAT-026</t>
+  </si>
+  <si>
+    <t>TP-BAT-027</t>
+  </si>
+  <si>
+    <t>TP-BAT-028</t>
+  </si>
+  <si>
+    <t>Cerrar interfaz de simulación</t>
+  </si>
+  <si>
+    <t>Cerrar aplicación principal</t>
+  </si>
+  <si>
+    <t>Con este y el siguiente paso, se procede a realizar el cierre de la aplicación para finalizar con la ejecución del procedimiento.</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es mayor que el límite establecido y la fuente de alimentación principal continua activa,
+Caso: NO falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es mayor que el límite establecido y la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería mayor que el límite (80%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa
+Caso: NO falla eléctrica y Nivel Batería mayor que el límite (80%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe continuar apagado debido a que el nivel de la batería de respaldo es mayor que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa,
+Caso: Falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a encendido (color verde)
+Nota: El LED debe encenderse debido a que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a encendido (color verde)
+Nota: El LED debe encenderse debido a que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a encendido (color verde)
+Nota: El LED debe encenderse debido a que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe apagarse debido a que el nivel de la batería de respaldo es mayor o igual que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe apagarse debido a que el nivel de la batería de respaldo es mayor o igual que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Batería" ya que aunque el nivel de la batería de respaldo es mayor o igual que el límite establecido, la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Verificar que el LED "Batería" es igual a apagado (no color)
+Nota: El LED debe apagarse debido a que el nivel de la batería de respaldo es mayor o igual que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería mayor al límite (80%)</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Principal"
+Nota: El Indicador de Fuente de alimentación debe indicar "Batería" ya que aunque el nivel de la batería de respaldo es mayor o igual que el límite establecido, la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería mayor a límite (80%)</t>
+  </si>
+  <si>
+    <t>Pasó</t>
+  </si>
+  <si>
+    <t>PRINCIPAL</t>
+  </si>
+  <si>
+    <t>Verificar que indicador "Fuente Alimentación" permanece igual a "Bateria"
+Nota: El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es mayor que el límite establecido pero la fuente de alimentación principal NO se encuentra activa
+Caso: Falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>BATERIA</t>
+  </si>
+  <si>
+    <t>ENCENDIDO</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>El LED debe continuar apagado debido a que el nivel de la batería de respaldo es mayor que el límite establecido y la fuente de alimentación principal continua activa</t>
+  </si>
+  <si>
+    <t>El LED debe continuar apagado debido a que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>El Indicador de Fuente de alimentación debe indicar "Principal" ya que el nivel de la batería de respaldo es menor que el límite establecido pero la fuente de alimentación principal continua activa</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Caso: NO falla eléctrica y Nivel Batería mayor que el límite (80%)</t>
+  </si>
+  <si>
+    <t>El LED debe encenderse debido a que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería mínimo</t>
+  </si>
+  <si>
+    <t>El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es menor que el límite establecido y la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería menor a límite (20%)</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería igual a límite-1 (49%)</t>
+  </si>
+  <si>
+    <t>El LED debe apagarse debido a que el nivel de la batería de respaldo es mayor o igual que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería igual a límite (50%)</t>
+  </si>
+  <si>
+    <t>El Indicador de Fuente de alimentación debe indicar "Batería" ya que aunque el nivel de la batería de respaldo es mayor o igual que el límite establecido, la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería máximo</t>
+  </si>
+  <si>
+    <t>El Indicador de Fuente de alimentación debe indicar "Bateria" ya que el nivel de la batería de respaldo es mayor que el límite establecido pero la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>El LED debe continuar apagado debido a que el nivel de la batería de respaldo es mayor que el límite establecido aunque la fuente de alimentación principal NO se encuentra activa</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería igual a límite+1 (51%)</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería mayor al límite (80%)</t>
+  </si>
+  <si>
+    <t>Caso: Falla eléctrica y Nivel Batería mayor a límite (80%)</t>
+  </si>
+  <si>
+    <t>NO FALLA EN RED ELECTRICA</t>
+  </si>
+  <si>
+    <t>SISTEMA EN OPERACIÓN NORMAL</t>
+  </si>
+  <si>
+    <t>FALLA EN RED ELECTRICA</t>
+  </si>
+  <si>
+    <t>Falla eléctrica OFF</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 100</t>
+  </si>
+  <si>
+    <t>Falla eléctrica ON</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 0</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 20</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 49</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 50</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 51</t>
+  </si>
+  <si>
+    <t>Voltaje Batería = 80</t>
+  </si>
+  <si>
+    <t>LED APAGADO</t>
+  </si>
+  <si>
+    <t>Indicador "Principal"</t>
+  </si>
+  <si>
+    <t>Indicador "Bateria"</t>
+  </si>
+  <si>
+    <t>LED ENCENDIDO</t>
+  </si>
+  <si>
+    <t>SW-ID-3
+SW-ID-11
+SW-ID-12</t>
+  </si>
+  <si>
+    <t>SW-ID-4
+SW-ID-19
+SW-ID-20</t>
+  </si>
+  <si>
+    <t>Borrador 9</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -286,6 +688,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="5">
     <fill>
@@ -313,7 +721,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -417,19 +825,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color theme="4"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="thin">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -456,8 +851,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -477,17 +873,19 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="1">
+  <dxfs count="2">
     <dxf>
-      <alignment horizontal="left" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -503,14 +901,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B12:F21" totalsRowShown="0">
-  <autoFilter ref="B12:F21" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="B12:F63" totalsRowShown="0">
+  <autoFilter ref="B12:F63" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="5">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Acción" dataDxfId="0"/>
     <tableColumn id="3" xr3:uid="{B14ED228-12A3-41C7-8F8D-4E780E61FC73}" name="ID"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Valor obtenido"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Resultado"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Comentario"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="Comentario" dataDxfId="1"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -803,27 +1201,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A2:M15"/>
+  <dimension ref="A2:M39"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView topLeftCell="A30" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F35" sqref="F35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20.85546875" customWidth="1"/>
     <col min="2" max="2" width="12.28515625" customWidth="1"/>
-    <col min="3" max="5" width="14" customWidth="1"/>
-    <col min="6" max="6" width="10.7109375" customWidth="1"/>
-    <col min="13" max="13" width="43.140625" customWidth="1"/>
+    <col min="3" max="3" width="42" customWidth="1"/>
+    <col min="4" max="5" width="14" customWidth="1"/>
+    <col min="6" max="7" width="10.7109375" customWidth="1"/>
+    <col min="11" max="11" width="10.28515625" customWidth="1"/>
+    <col min="12" max="12" width="9.7109375" customWidth="1"/>
+    <col min="13" max="13" width="54.140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="4" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="C2" s="3"/>
       <c r="D2" s="3"/>
@@ -831,10 +1232,10 @@
     </row>
     <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -842,10 +1243,10 @@
     </row>
     <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -853,10 +1254,10 @@
     </row>
     <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="4" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C5" s="3"/>
       <c r="D5" s="3"/>
@@ -864,10 +1265,10 @@
     </row>
     <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C6" s="3"/>
       <c r="D6" s="3"/>
@@ -875,10 +1276,10 @@
     </row>
     <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C7" s="3"/>
       <c r="D7" s="3"/>
@@ -886,190 +1287,1251 @@
     </row>
     <row r="8" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="9" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="B9" s="10" t="s">
+      <c r="B9" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="C9" s="10" t="s">
+      <c r="C9" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="D9" s="10" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" s="10" t="s">
-        <v>34</v>
-      </c>
-      <c r="F9" s="13" t="s">
+      <c r="D9" s="11" t="s">
+        <v>31</v>
+      </c>
+      <c r="E9" s="11" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="G9" s="14"/>
-      <c r="H9" s="14"/>
-      <c r="I9" s="14"/>
-      <c r="J9" s="14"/>
-      <c r="K9" s="14"/>
-      <c r="L9" s="15"/>
-      <c r="M9" s="10" t="s">
+      <c r="G9" s="15"/>
+      <c r="H9" s="15"/>
+      <c r="I9" s="15"/>
+      <c r="J9" s="15"/>
+      <c r="K9" s="15"/>
+      <c r="L9" s="16"/>
+      <c r="M9" s="11" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="10" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A10" s="11"/>
-      <c r="B10" s="11"/>
-      <c r="C10" s="11"/>
-      <c r="D10" s="11"/>
-      <c r="E10" s="11"/>
-      <c r="F10" s="13" t="s">
+      <c r="A10" s="12"/>
+      <c r="B10" s="12"/>
+      <c r="C10" s="12"/>
+      <c r="D10" s="12"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="G10" s="15"/>
-      <c r="H10" s="13" t="s">
+      <c r="G10" s="16"/>
+      <c r="H10" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="I10" s="14"/>
-      <c r="J10" s="15"/>
-      <c r="K10" s="13" t="s">
-        <v>26</v>
-      </c>
-      <c r="L10" s="15"/>
-      <c r="M10" s="11"/>
+      <c r="I10" s="15"/>
+      <c r="J10" s="16"/>
+      <c r="K10" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="L10" s="16"/>
+      <c r="M10" s="12"/>
     </row>
     <row r="11" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A11" s="12"/>
-      <c r="B11" s="12"/>
-      <c r="C11" s="12"/>
-      <c r="D11" s="12"/>
-      <c r="E11" s="12"/>
+      <c r="A11" s="13"/>
+      <c r="B11" s="13"/>
+      <c r="C11" s="13"/>
+      <c r="D11" s="13"/>
+      <c r="E11" s="13"/>
       <c r="F11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="H11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="G11" s="6" t="s">
+      <c r="I11" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="H11" s="6" t="s">
+      <c r="J11" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="I11" s="6" t="s">
+      <c r="K11" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="J11" s="6" t="s">
+      <c r="L11" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="K11" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="L11" s="6" t="s">
-        <v>15</v>
-      </c>
-      <c r="M11" s="12"/>
-    </row>
-    <row r="12" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="M11" s="13"/>
+    </row>
+    <row r="12" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
-        <v>7</v>
+        <v>61</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C12" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="D12" s="2" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
       <c r="E12" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M12" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="F12" s="2"/>
-      <c r="G12" s="2"/>
-      <c r="H12" s="2"/>
-      <c r="I12" s="2"/>
-      <c r="J12" s="2"/>
-      <c r="K12" s="2"/>
-      <c r="L12" s="2"/>
-      <c r="M12" s="2"/>
-    </row>
-    <row r="13" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A13" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="B13" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C13" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>142</v>
+      </c>
       <c r="D13" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F13" s="2"/>
-      <c r="G13" s="2"/>
-      <c r="H13" s="2"/>
-      <c r="I13" s="2"/>
-      <c r="J13" s="2"/>
-      <c r="K13" s="2"/>
-      <c r="L13" s="2"/>
-      <c r="M13" s="2"/>
-    </row>
-    <row r="14" spans="1:13" ht="26.25" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J13" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K13" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L13" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M13" s="2" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C14" s="2"/>
+        <v>182</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>143</v>
+      </c>
       <c r="D14" s="2" t="s">
-        <v>60</v>
+        <v>55</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="2"/>
-      <c r="G14" s="2"/>
-      <c r="H14" s="2"/>
-      <c r="I14" s="2"/>
-      <c r="J14" s="2"/>
-      <c r="K14" s="2"/>
-      <c r="L14" s="2"/>
-      <c r="M14" s="2"/>
-    </row>
-    <row r="15" spans="1:13" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+        <v>58</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J14" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L14" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M14" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
-        <v>7</v>
+        <v>85</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
-      <c r="G15" s="2"/>
-      <c r="H15" s="2"/>
-      <c r="I15" s="2"/>
-      <c r="J15" s="2"/>
-      <c r="K15" s="2"/>
-      <c r="L15" s="2"/>
-      <c r="M15" s="2"/>
+        <v>181</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J15" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L15" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M15" s="2" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K16" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L16" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M16" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J17" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K17" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L17" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M17" s="2" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A18" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K18" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L18" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M18" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A19" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J19" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K19" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L19" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M19" s="2" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K20" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L20" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M20" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A21" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M21" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K22" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L22" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M22" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A23" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M23" s="2" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A24" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I24" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K24" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L24" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M24" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A25" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>145</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E25" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F25" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="G25" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H25" s="2" t="s">
+        <v>168</v>
+      </c>
+      <c r="I25" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J25" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K25" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L25" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="M25" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>161</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E26" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H26" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M26" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>160</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H27" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>169</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="B28" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E28" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F28" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G28" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K28" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M28" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B29" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C29" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="E29" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F29" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G29" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H29" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I29" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J29" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K29" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L29" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M29" s="2" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B30" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C30" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E30" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F30" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G30" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H30" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K30" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L30" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M30" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B31" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C31" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F31" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G31" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H31" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="J31" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K31" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L31" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M31" s="2" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B32" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C32" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="D32" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E32" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F32" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G32" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H32" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L32" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B33" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C33" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="D33" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E33" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F33" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G33" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H33" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>173</v>
+      </c>
+      <c r="J33" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K33" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="L33" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M33" s="2" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C34" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D34" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F34" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G34" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H34" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K34" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L34" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M34" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="1" t="s">
+        <v>105</v>
+      </c>
+      <c r="B35" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C35" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D35" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F35" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G35" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H35" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>174</v>
+      </c>
+      <c r="J35" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K35" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L35" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M35" s="2" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B36" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C36" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E36" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F36" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G36" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H36" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K36" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L36" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M36" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A37" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C37" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E37" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="F37" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G37" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H37" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>175</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L37" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" ht="51.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>182</v>
+      </c>
+      <c r="C38" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="D38" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E38" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F38" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G38" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H38" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K38" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M38" s="2" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="64.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>181</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>158</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E39" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>167</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="H39" s="2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I39" s="2" t="s">
+        <v>176</v>
+      </c>
+      <c r="J39" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="K39" s="2" t="s">
+        <v>177</v>
+      </c>
+      <c r="L39" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>164</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">
+    <mergeCell ref="E9:E11"/>
+    <mergeCell ref="D9:D11"/>
+    <mergeCell ref="C9:C11"/>
+    <mergeCell ref="A9:A11"/>
+    <mergeCell ref="B9:B11"/>
     <mergeCell ref="M9:M11"/>
     <mergeCell ref="F9:L9"/>
     <mergeCell ref="F10:G10"/>
     <mergeCell ref="H10:J10"/>
     <mergeCell ref="K10:L10"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D9:D11"/>
-    <mergeCell ref="C9:C11"/>
-    <mergeCell ref="A9:A11"/>
-    <mergeCell ref="B9:B11"/>
   </mergeCells>
-  <dataValidations count="2">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D15" xr:uid="{00000000-0002-0000-0000-000000000000}">
+  <phoneticPr fontId="5" type="noConversion"/>
+  <dataValidations disablePrompts="1" count="2">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D12:D39" xr:uid="{00000000-0002-0000-0000-000000000000}">
       <formula1>"Normal, Robustez"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E15" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E12:E39" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"Valor de frontera, Clase Equivalencia, Maq. Estados Finitos, Expresión Booleana, Otro"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1080,10 +2542,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A2:F26"/>
+  <dimension ref="A2:F65"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1098,28 +2560,28 @@
   <sheetData>
     <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B2" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B3" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B4" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="C4" s="17"/>
+        <v>26</v>
+      </c>
+      <c r="B4" s="10" t="s">
+        <v>44</v>
+      </c>
+      <c r="C4" s="10"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
@@ -1128,57 +2590,57 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>39</v>
+      </c>
+      <c r="B6" t="s">
         <v>42</v>
-      </c>
-      <c r="B6" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>37</v>
-      </c>
-      <c r="B7" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C7" s="16"/>
+        <v>35</v>
+      </c>
+      <c r="B7" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="C7" s="9"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>45</v>
+        <v>183</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B9" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B12" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="E12" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="F12" t="s">
         <v>4</v>
@@ -1188,129 +2650,835 @@
       <c r="A13" s="8">
         <v>1</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
+      <c r="B13" s="10" t="s">
+        <v>45</v>
       </c>
       <c r="D13" t="s">
-        <v>50</v>
-      </c>
-      <c r="F13" s="17" t="s">
-        <v>52</v>
+        <v>46</v>
+      </c>
+      <c r="F13" s="10" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14" s="8">
         <v>2</v>
       </c>
-      <c r="B14" t="s">
-        <v>53</v>
+      <c r="B14" s="10" t="s">
+        <v>48</v>
       </c>
       <c r="D14" t="s">
-        <v>50</v>
-      </c>
+        <v>46</v>
+      </c>
+      <c r="F14" s="10"/>
     </row>
     <row r="15" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="8">
         <v>3</v>
       </c>
-      <c r="B15" t="s">
-        <v>54</v>
+      <c r="B15" s="10" t="s">
+        <v>49</v>
       </c>
       <c r="D15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F15" s="10" t="s">
         <v>50</v>
       </c>
-      <c r="F15" s="17" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="8">
         <v>4</v>
       </c>
-      <c r="B16" t="s">
-        <v>56</v>
+      <c r="B16" s="10" t="s">
+        <v>51</v>
       </c>
       <c r="D16" t="s">
-        <v>50</v>
+        <v>46</v>
+      </c>
+      <c r="F16" s="10" t="s">
+        <v>63</v>
       </c>
     </row>
     <row r="17" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A17" s="8">
         <v>5</v>
       </c>
-      <c r="B17" t="s">
-        <v>57</v>
+      <c r="B17" s="10" t="s">
+        <v>52</v>
       </c>
       <c r="D17" t="s">
-        <v>50</v>
-      </c>
-      <c r="F17" s="17" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F17" s="10" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A18" s="8">
         <v>6</v>
       </c>
-      <c r="B18" t="s">
-        <v>59</v>
+      <c r="B18" s="10" t="s">
+        <v>64</v>
       </c>
       <c r="D18" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F18" s="10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="8">
         <v>7</v>
       </c>
-      <c r="B19" t="s">
-        <v>64</v>
-      </c>
-      <c r="C19" t="s">
-        <v>68</v>
+      <c r="B19" s="10" t="s">
+        <v>54</v>
       </c>
       <c r="D19" t="s">
-        <v>67</v>
-      </c>
-      <c r="E19" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>46</v>
+      </c>
+      <c r="F19" s="10" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="8">
         <v>8</v>
       </c>
-      <c r="B20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" s="9">
+      <c r="B20" s="10" t="s">
+        <v>113</v>
+      </c>
+      <c r="C20" t="s">
+        <v>61</v>
+      </c>
+      <c r="D20" t="s">
+        <v>60</v>
+      </c>
+      <c r="E20" t="s">
+        <v>136</v>
+      </c>
+      <c r="F20" s="10"/>
+    </row>
+    <row r="21" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A21" s="8">
         <v>9</v>
       </c>
-      <c r="B21" t="s">
+      <c r="B21" s="10" t="s">
+        <v>114</v>
+      </c>
+      <c r="C21" t="s">
+        <v>62</v>
+      </c>
+      <c r="D21" t="s">
+        <v>137</v>
+      </c>
+      <c r="E21" t="s">
+        <v>136</v>
+      </c>
+      <c r="F21" s="10"/>
+    </row>
+    <row r="22" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="8">
+        <v>10</v>
+      </c>
+      <c r="B22" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D22" t="s">
+        <v>46</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="23" spans="1:6" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A23" s="8">
+        <v>11</v>
+      </c>
+      <c r="B23" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="C23" t="s">
+        <v>84</v>
+      </c>
+      <c r="D23" t="s">
+        <v>60</v>
+      </c>
+      <c r="E23" t="s">
+        <v>136</v>
+      </c>
+      <c r="F23" s="10"/>
+    </row>
+    <row r="24" spans="1:6" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="8">
+        <v>12</v>
+      </c>
+      <c r="B24" s="10" t="s">
+        <v>116</v>
+      </c>
+      <c r="C24" t="s">
+        <v>85</v>
+      </c>
+      <c r="D24" t="s">
+        <v>137</v>
+      </c>
+      <c r="E24" t="s">
+        <v>136</v>
+      </c>
+      <c r="F24" s="10"/>
+    </row>
+    <row r="25" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="8">
+        <v>13</v>
+      </c>
+      <c r="B25" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D25" t="s">
+        <v>46</v>
+      </c>
+      <c r="F25" s="10" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="26" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A26" s="8">
+        <v>14</v>
+      </c>
+      <c r="B26" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="C26" t="s">
+        <v>86</v>
+      </c>
+      <c r="D26" t="s">
+        <v>60</v>
+      </c>
+      <c r="E26" t="s">
+        <v>136</v>
+      </c>
+      <c r="F26" s="10"/>
+    </row>
+    <row r="27" spans="1:6" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="8">
+        <v>15</v>
+      </c>
+      <c r="B27" s="10" t="s">
+        <v>118</v>
+      </c>
+      <c r="C27" t="s">
+        <v>87</v>
+      </c>
+      <c r="D27" t="s">
+        <v>137</v>
+      </c>
+      <c r="E27" t="s">
+        <v>136</v>
+      </c>
+      <c r="F27" s="10"/>
+    </row>
+    <row r="28" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="8">
+        <v>16</v>
+      </c>
+      <c r="B28" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D28" t="s">
+        <v>46</v>
+      </c>
+      <c r="F28" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="29" spans="1:6" ht="105" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="8">
+        <v>17</v>
+      </c>
+      <c r="B29" s="10" t="s">
+        <v>119</v>
+      </c>
+      <c r="C29" t="s">
+        <v>88</v>
+      </c>
+      <c r="D29" t="s">
+        <v>60</v>
+      </c>
+      <c r="E29" t="s">
+        <v>136</v>
+      </c>
+      <c r="F29" s="10"/>
+    </row>
+    <row r="30" spans="1:6" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="8">
+        <v>18</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>120</v>
+      </c>
+      <c r="C30" t="s">
+        <v>89</v>
+      </c>
+      <c r="D30" t="s">
+        <v>137</v>
+      </c>
+      <c r="E30" t="s">
+        <v>136</v>
+      </c>
+      <c r="F30" s="10"/>
+    </row>
+    <row r="31" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="8">
+        <v>19</v>
+      </c>
+      <c r="B31" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D31" t="s">
+        <v>46</v>
+      </c>
+      <c r="F31" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="32" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="8">
+        <v>20</v>
+      </c>
+      <c r="B32" s="10" t="s">
+        <v>121</v>
+      </c>
+      <c r="C32" t="s">
+        <v>90</v>
+      </c>
+      <c r="D32" t="s">
+        <v>60</v>
+      </c>
+      <c r="E32" t="s">
+        <v>136</v>
+      </c>
+      <c r="F32" s="10"/>
+    </row>
+    <row r="33" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="8">
+        <v>21</v>
+      </c>
+      <c r="B33" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="C33" t="s">
+        <v>91</v>
+      </c>
+      <c r="D33" t="s">
+        <v>137</v>
+      </c>
+      <c r="E33" t="s">
+        <v>136</v>
+      </c>
+      <c r="F33" s="10"/>
+    </row>
+    <row r="34" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="8">
+        <v>22</v>
+      </c>
+      <c r="B34" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D34" t="s">
+        <v>46</v>
+      </c>
+      <c r="F34" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="35" spans="1:6" ht="108.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A35" s="8">
+        <v>23</v>
+      </c>
+      <c r="B35" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="C35" t="s">
+        <v>92</v>
+      </c>
+      <c r="D35" t="s">
+        <v>60</v>
+      </c>
+      <c r="E35" t="s">
+        <v>136</v>
+      </c>
+      <c r="F35" s="10"/>
+    </row>
+    <row r="36" spans="1:6" ht="119.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A36" s="8">
+        <v>24</v>
+      </c>
+      <c r="B36" s="17" t="s">
+        <v>124</v>
+      </c>
+      <c r="C36" t="s">
+        <v>93</v>
+      </c>
+      <c r="D36" t="s">
+        <v>137</v>
+      </c>
+      <c r="E36" t="s">
+        <v>136</v>
+      </c>
+      <c r="F36" s="10"/>
+    </row>
+    <row r="37" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A37" s="8">
+        <v>25</v>
+      </c>
+      <c r="B37" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D37" t="s">
+        <v>46</v>
+      </c>
+      <c r="F37" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="38" spans="1:6" ht="121.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="8">
+        <v>26</v>
+      </c>
+      <c r="B38" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="C38" t="s">
+        <v>94</v>
+      </c>
+      <c r="D38" t="s">
+        <v>60</v>
+      </c>
+      <c r="E38" t="s">
+        <v>136</v>
+      </c>
+      <c r="F38" s="10"/>
+    </row>
+    <row r="39" spans="1:6" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="8">
+        <v>27</v>
+      </c>
+      <c r="B39" s="17" t="s">
+        <v>126</v>
+      </c>
+      <c r="C39" t="s">
+        <v>95</v>
+      </c>
+      <c r="D39" t="s">
+        <v>137</v>
+      </c>
+      <c r="E39" t="s">
+        <v>136</v>
+      </c>
+      <c r="F39" s="10"/>
+    </row>
+    <row r="40" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+      <c r="A40" s="8">
+        <v>28</v>
+      </c>
+      <c r="B40" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="D40" t="s">
+        <v>46</v>
+      </c>
+      <c r="F40" s="10" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="41" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="8">
+        <v>29</v>
+      </c>
+      <c r="B41" s="10" t="s">
+        <v>54</v>
+      </c>
+      <c r="D41" t="s">
+        <v>46</v>
+      </c>
+      <c r="F41" s="10" t="s">
         <v>66</v>
       </c>
-      <c r="C21" t="s">
+    </row>
+    <row r="42" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A42" s="8">
+        <v>30</v>
+      </c>
+      <c r="B42" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="C42" t="s">
+        <v>96</v>
+      </c>
+      <c r="D42" t="s">
+        <v>60</v>
+      </c>
+      <c r="E42" t="s">
+        <v>136</v>
+      </c>
+      <c r="F42" s="10"/>
+    </row>
+    <row r="43" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A43" s="8">
+        <v>31</v>
+      </c>
+      <c r="B43" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="C43" t="s">
+        <v>97</v>
+      </c>
+      <c r="D43" t="s">
+        <v>139</v>
+      </c>
+      <c r="E43" t="s">
+        <v>136</v>
+      </c>
+      <c r="F43" s="10"/>
+    </row>
+    <row r="44" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A44" s="8">
+        <v>32</v>
+      </c>
+      <c r="B44" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="D44" t="s">
+        <v>46</v>
+      </c>
+      <c r="F44" s="10" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="45" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A45" s="8">
+        <v>33</v>
+      </c>
+      <c r="B45" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="C45" t="s">
+        <v>98</v>
+      </c>
+      <c r="D45" t="s">
+        <v>140</v>
+      </c>
+      <c r="E45" t="s">
+        <v>136</v>
+      </c>
+      <c r="F45" s="10"/>
+    </row>
+    <row r="46" spans="1:6" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="8">
+        <v>34</v>
+      </c>
+      <c r="B46" s="10" t="s">
+        <v>81</v>
+      </c>
+      <c r="C46" t="s">
+        <v>99</v>
+      </c>
+      <c r="D46" t="s">
+        <v>139</v>
+      </c>
+      <c r="E46" t="s">
+        <v>136</v>
+      </c>
+      <c r="F46" s="10"/>
+    </row>
+    <row r="47" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A47" s="8">
+        <v>35</v>
+      </c>
+      <c r="B47" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="D47" t="s">
+        <v>46</v>
+      </c>
+      <c r="F47" s="10" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B22" s="5"/>
-      <c r="C22" s="5"/>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B23" s="5"/>
-      <c r="C23" s="5"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+    <row r="48" spans="1:6" ht="105" x14ac:dyDescent="0.25">
+      <c r="A48" s="8">
+        <v>36</v>
+      </c>
+      <c r="B48" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="C48" t="s">
+        <v>100</v>
+      </c>
+      <c r="D48" t="s">
+        <v>140</v>
+      </c>
+      <c r="E48" t="s">
+        <v>136</v>
+      </c>
+      <c r="F48" s="10"/>
+    </row>
+    <row r="49" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A49" s="8">
+        <v>37</v>
+      </c>
+      <c r="B49" s="10" t="s">
+        <v>82</v>
+      </c>
+      <c r="C49" t="s">
+        <v>101</v>
+      </c>
+      <c r="D49" t="s">
+        <v>139</v>
+      </c>
+      <c r="E49" t="s">
+        <v>136</v>
+      </c>
+      <c r="F49" s="10"/>
+    </row>
+    <row r="50" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A50" s="8">
+        <v>38</v>
+      </c>
+      <c r="B50" s="10" t="s">
+        <v>70</v>
+      </c>
+      <c r="D50" t="s">
+        <v>46</v>
+      </c>
+      <c r="F50" s="10" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="51" spans="1:6" ht="108" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A51" s="8">
+        <v>39</v>
+      </c>
+      <c r="B51" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="C51" t="s">
+        <v>102</v>
+      </c>
+      <c r="D51" t="s">
+        <v>140</v>
+      </c>
+      <c r="E51" t="s">
+        <v>136</v>
+      </c>
+      <c r="F51" s="10"/>
+    </row>
+    <row r="52" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A52" s="8">
+        <v>40</v>
+      </c>
+      <c r="B52" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="C52" t="s">
+        <v>103</v>
+      </c>
+      <c r="D52" t="s">
+        <v>139</v>
+      </c>
+      <c r="E52" t="s">
+        <v>136</v>
+      </c>
+      <c r="F52" s="10"/>
+    </row>
+    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A53" s="8">
         <v>41</v>
       </c>
+      <c r="B53" s="10" t="s">
+        <v>72</v>
+      </c>
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+      <c r="F53" s="10" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="54" spans="1:6" ht="106.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="8">
+        <v>42</v>
+      </c>
+      <c r="B54" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="C54" t="s">
+        <v>104</v>
+      </c>
+      <c r="D54" t="s">
+        <v>60</v>
+      </c>
+      <c r="E54" t="s">
+        <v>136</v>
+      </c>
+      <c r="F54" s="10"/>
+    </row>
+    <row r="55" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A55" s="8">
+        <v>43</v>
+      </c>
+      <c r="B55" s="17" t="s">
+        <v>80</v>
+      </c>
+      <c r="C55" t="s">
+        <v>105</v>
+      </c>
+      <c r="D55" t="s">
+        <v>139</v>
+      </c>
+      <c r="E55" t="s">
+        <v>136</v>
+      </c>
+      <c r="F55" s="10"/>
+    </row>
+    <row r="56" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A56" s="8">
+        <v>44</v>
+      </c>
+      <c r="B56" s="10" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" t="s">
+        <v>46</v>
+      </c>
+      <c r="F56" s="10" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="57" spans="1:6" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="8">
+        <v>45</v>
+      </c>
+      <c r="B57" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="C57" t="s">
+        <v>106</v>
+      </c>
+      <c r="D57" t="s">
+        <v>60</v>
+      </c>
+      <c r="E57" t="s">
+        <v>136</v>
+      </c>
+      <c r="F57" s="10"/>
+    </row>
+    <row r="58" spans="1:6" ht="120" x14ac:dyDescent="0.25">
+      <c r="A58" s="8">
+        <v>46</v>
+      </c>
+      <c r="B58" s="17" t="s">
+        <v>133</v>
+      </c>
+      <c r="C58" t="s">
+        <v>107</v>
+      </c>
+      <c r="D58" t="s">
+        <v>139</v>
+      </c>
+      <c r="E58" t="s">
+        <v>136</v>
+      </c>
+      <c r="F58" s="10"/>
+    </row>
+    <row r="59" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+      <c r="A59" s="8">
+        <v>47</v>
+      </c>
+      <c r="B59" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="D59" t="s">
+        <v>46</v>
+      </c>
+      <c r="F59" s="10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="60" spans="1:6" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="8">
+        <v>48</v>
+      </c>
+      <c r="B60" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="C60" t="s">
+        <v>108</v>
+      </c>
+      <c r="D60" t="s">
+        <v>60</v>
+      </c>
+      <c r="E60" t="s">
+        <v>136</v>
+      </c>
+      <c r="F60" s="10"/>
+    </row>
+    <row r="61" spans="1:6" ht="120.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="8">
+        <v>49</v>
+      </c>
+      <c r="B61" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="C61" t="s">
+        <v>109</v>
+      </c>
+      <c r="D61" t="s">
+        <v>139</v>
+      </c>
+      <c r="E61" t="s">
+        <v>136</v>
+      </c>
+      <c r="F61" s="10"/>
+    </row>
+    <row r="62" spans="1:6" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="8">
+        <v>50</v>
+      </c>
+      <c r="B62" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="D62" t="s">
+        <v>46</v>
+      </c>
+      <c r="F62" s="10" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A63" s="8">
+        <v>51</v>
+      </c>
+      <c r="B63" s="10" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63" t="s">
+        <v>46</v>
+      </c>
+      <c r="F63" s="10"/>
+    </row>
+    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B64" s="5"/>
+      <c r="C64" s="5"/>
+    </row>
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B65" s="5"/>
+      <c r="C65" s="5"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E23" xr:uid="{00000000-0002-0000-0100-000000000000}">
+  <dataValidations disablePrompts="1" count="1">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="E13:E65" xr:uid="{00000000-0002-0000-0100-000000000000}">
       <formula1>"Pasó, Falló"</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>